<commit_message>
Continuing work on utilities
</commit_message>
<xml_diff>
--- a/PinAssignments.xlsx
+++ b/PinAssignments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\ESP32\projects\TVLift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6351BA7-A969-4C53-AC86-0429023B27AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5968CDC-51C0-42F0-85EF-3E0902B311C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5A3BED3-B86A-457C-90DE-18F9FEEAD38D}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,17 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Lift ENA</t>
   </si>
   <si>
-    <t>Lift DIR</t>
-  </si>
-  <si>
-    <t>Lift PUL</t>
-  </si>
-  <si>
     <t>SPI</t>
   </si>
   <si>
@@ -55,6 +50,24 @@
   </si>
   <si>
     <t>Z+ Endstop</t>
+  </si>
+  <si>
+    <t>SPI CS</t>
+  </si>
+  <si>
+    <t>SPI MOSI</t>
+  </si>
+  <si>
+    <t>SPI MISO</t>
+  </si>
+  <si>
+    <t>SPI CLK</t>
+  </si>
+  <si>
+    <t>Lift Pul</t>
+  </si>
+  <si>
+    <t>Lift Dir</t>
   </si>
 </sst>
 </file>
@@ -493,7 +506,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,44 +518,57 @@
   <sheetData>
     <row r="1" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O2" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="O3" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="N6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>